<commit_message>
Update PlayerInfo And Abandon  Something
更新人物属性以及删除不必要的脚本
</commit_message>
<xml_diff>
--- a/PlayerRoleInfo.xlsx
+++ b/PlayerRoleInfo.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\15271\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30EC1A46-4518-4859-876A-FC8310C2ED61}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1005" yWindow="-120" windowWidth="19605" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1008" yWindow="-120" windowWidth="19608" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="44">
   <si>
     <t>RoleId</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -106,10 +100,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1,2,3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>4,5,6</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -179,14 +169,38 @@
   </si>
   <si>
     <t>速度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int[]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>float</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[1,2,3]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.8f</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -284,7 +298,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -319,7 +333,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -496,32 +510,32 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K1:K5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="5" width="9" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="14.625" customWidth="1"/>
-    <col min="12" max="12" width="12.75" customWidth="1"/>
-    <col min="13" max="13" width="14.375" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" customWidth="1"/>
+    <col min="12" max="12" width="12.77734375" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -532,13 +546,13 @@
         <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
         <v>6</v>
@@ -553,197 +567,244 @@
         <v>18</v>
       </c>
       <c r="K1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
         <v>38</v>
       </c>
       <c r="F2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" t="s">
+        <v>41</v>
+      </c>
+      <c r="O2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" t="s">
         <v>7</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H3" t="s">
         <v>8</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I3" t="s">
         <v>10</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J3" t="s">
         <v>17</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K3" t="s">
         <v>19</v>
       </c>
-      <c r="L2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N2" t="s">
-        <v>29</v>
-      </c>
-      <c r="O2" t="s">
-        <v>31</v>
+      <c r="L3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O3" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="4" spans="1:15">
+      <c r="A4">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="D3">
+      <c r="D4">
         <v>65</v>
       </c>
-      <c r="E3">
+      <c r="E4">
         <v>50</v>
       </c>
-      <c r="F3">
+      <c r="F4">
         <v>100</v>
       </c>
-      <c r="G3">
+      <c r="G4">
         <v>60</v>
       </c>
-      <c r="H3">
+      <c r="H4">
         <v>30</v>
       </c>
-      <c r="I3">
+      <c r="I4">
         <v>3</v>
       </c>
-      <c r="J3">
+      <c r="J4">
         <v>7</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L4">
+        <v>3</v>
+      </c>
+      <c r="N4">
+        <v>0.08</v>
+      </c>
+      <c r="O4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5">
+        <v>70</v>
+      </c>
+      <c r="E5">
+        <v>45</v>
+      </c>
+      <c r="F5">
+        <v>500</v>
+      </c>
+      <c r="G5">
+        <v>80</v>
+      </c>
+      <c r="H5">
+        <v>10</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>8</v>
+      </c>
+      <c r="K5" t="s">
         <v>20</v>
       </c>
-      <c r="L3">
+      <c r="L5">
+        <v>5</v>
+      </c>
+      <c r="N5">
+        <v>0.1</v>
+      </c>
+      <c r="O5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6">
         <v>3</v>
       </c>
-      <c r="N3">
-        <v>0.08</v>
-      </c>
-      <c r="O3">
-        <v>4.8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4">
-        <v>70</v>
-      </c>
-      <c r="E4">
-        <v>45</v>
-      </c>
-      <c r="F4">
-        <v>500</v>
-      </c>
-      <c r="G4">
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6">
         <v>80</v>
       </c>
-      <c r="H4">
-        <v>10</v>
-      </c>
-      <c r="I4">
-        <v>2</v>
-      </c>
-      <c r="J4">
-        <v>8</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="E6">
+        <v>60</v>
+      </c>
+      <c r="F6">
+        <v>300</v>
+      </c>
+      <c r="G6">
+        <v>50</v>
+      </c>
+      <c r="H6">
+        <v>50</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6" t="s">
         <v>21</v>
       </c>
-      <c r="L4">
-        <v>5</v>
-      </c>
-      <c r="N4">
-        <v>0.1</v>
-      </c>
-      <c r="O4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5">
-        <v>80</v>
-      </c>
-      <c r="E5">
-        <v>60</v>
-      </c>
-      <c r="F5">
-        <v>300</v>
-      </c>
-      <c r="G5">
-        <v>50</v>
-      </c>
-      <c r="H5">
-        <v>50</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L5">
+      <c r="L6">
         <v>6</v>
       </c>
-      <c r="N5">
+      <c r="N6">
         <v>0.15</v>
       </c>
-      <c r="O5">
+      <c r="O6">
         <v>7.5</v>
       </c>
     </row>

</xml_diff>